<commit_message>
mensagem clara sobre o que foi alterado
</commit_message>
<xml_diff>
--- a/Base/Backlog_19.xlsx
+++ b/Base/Backlog_19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\franciscoj\Python_Initial\Pyhton_Web\Base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB223E7-3736-446D-8F60-6FA8C9DF0151}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A963E5D-DAEA-415D-A82C-D23BC1E530EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="418" xr2:uid="{89A3EF9E-2AF9-420D-85DF-9BB5B68F651F}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="418" activeTab="1" xr2:uid="{89A3EF9E-2AF9-420D-85DF-9BB5B68F651F}"/>
   </bookViews>
   <sheets>
     <sheet name="ITI" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="26">
   <si>
     <t>Backlog</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Erick da Silva</t>
+  </si>
+  <si>
+    <t>Resolvido</t>
   </si>
 </sst>
 </file>
@@ -571,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69362A46-9E44-40AB-81A2-018EE27C1DC6}">
   <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -656,7 +659,7 @@
         <v>45789</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>11</v>
@@ -691,7 +694,7 @@
         <v>45789</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>11</v>
@@ -761,7 +764,7 @@
         <v>45789</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>11</v>
@@ -831,7 +834,7 @@
         <v>45789</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>11</v>
@@ -936,7 +939,7 @@
         <v>45789</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>11</v>
@@ -971,7 +974,7 @@
         <v>45789</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="K11" s="10" t="s">
         <v>11</v>
@@ -1006,7 +1009,7 @@
         <v>45789</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>11</v>
@@ -1111,7 +1114,7 @@
         <v>45789</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="K15" s="10" t="s">
         <v>11</v>
@@ -1539,8 +1542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A6A408-5BF6-4E16-8C71-EC6EB1F5A842}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C20" sqref="C19:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1623,7 +1626,7 @@
         <v>45782</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>15</v>
@@ -1658,7 +1661,7 @@
         <v>45782</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>15</v>

</xml_diff>